<commit_message>
liger_subcluster_complexheatmap: add marker genes
Former-commit-id: 83cc03e5828d06f5f5f1bfb71c7e837bbc82aafb
</commit_message>
<xml_diff>
--- a/resources/CelltypeMarkers_biologicalGroupings.xlsx
+++ b/resources/CelltypeMarkers_biologicalGroupings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LOChen/orion/nucseq_nd_dpolioud/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2449125-3EB8-7B42-AC39-0C900B08ED5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886DE464-E150-9F47-A245-A84EA9F019DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="16000" tabRatio="500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14400" windowHeight="15880" tabRatio="500" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="astrocytes_" sheetId="1" r:id="rId1"/>
@@ -22,9 +22,9 @@
     <sheet name="combined_markers" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">combined_markers!$A$1:$C$291</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">combined_markers!$A$1:$C$312</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1637" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="359">
   <si>
     <t>GENE</t>
   </si>
@@ -1021,6 +1021,96 @@
   </si>
   <si>
     <t>RTN4</t>
+  </si>
+  <si>
+    <t>COL12A1</t>
+  </si>
+  <si>
+    <t>MEG3</t>
+  </si>
+  <si>
+    <t>PSAP</t>
+  </si>
+  <si>
+    <t>NNAT</t>
+  </si>
+  <si>
+    <t>ATP1B1</t>
+  </si>
+  <si>
+    <t>FTH1</t>
+  </si>
+  <si>
+    <t>CALM1</t>
+  </si>
+  <si>
+    <t>PCHD15</t>
+  </si>
+  <si>
+    <t>NRXN1</t>
+  </si>
+  <si>
+    <t>TIAM1</t>
+  </si>
+  <si>
+    <t>NRCAM</t>
+  </si>
+  <si>
+    <t>LRP1B</t>
+  </si>
+  <si>
+    <t>KCNIP4</t>
+  </si>
+  <si>
+    <t>LRP1</t>
+  </si>
+  <si>
+    <t>PIP4K2A</t>
+  </si>
+  <si>
+    <t>PTPRD</t>
+  </si>
+  <si>
+    <t>PDE4B</t>
+  </si>
+  <si>
+    <t>LRRC7</t>
+  </si>
+  <si>
+    <t>TNR</t>
+  </si>
+  <si>
+    <t>DSCAM</t>
+  </si>
+  <si>
+    <t>NCOA1</t>
+  </si>
+  <si>
+    <t>CAMK2D</t>
+  </si>
+  <si>
+    <t>TMSB4X</t>
+  </si>
+  <si>
+    <t>TMSB10</t>
+  </si>
+  <si>
+    <t>PTMA</t>
+  </si>
+  <si>
+    <t>IFITM2</t>
+  </si>
+  <si>
+    <t>APT10A</t>
+  </si>
+  <si>
+    <t>ABCB1</t>
+  </si>
+  <si>
+    <t>PTPRG</t>
+  </si>
+  <si>
+    <t>GALNT18</t>
   </si>
 </sst>
 </file>
@@ -4578,10 +4668,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:C291"/>
+  <dimension ref="A1:C328"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A173" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F186" sqref="F186"/>
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G132" sqref="G132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.5" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5806,7 +5896,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
         <v>309</v>
       </c>
@@ -5814,7 +5904,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
         <v>310</v>
       </c>
@@ -5822,7 +5912,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
         <v>141</v>
       </c>
@@ -5830,7 +5920,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
         <v>311</v>
       </c>
@@ -5838,7 +5928,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
         <v>312</v>
       </c>
@@ -5846,7 +5936,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
         <v>313</v>
       </c>
@@ -5854,7 +5944,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
         <v>314</v>
       </c>
@@ -5862,7 +5952,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
         <v>315</v>
       </c>
@@ -5870,7 +5960,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
         <v>316</v>
       </c>
@@ -5878,7 +5968,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
         <v>317</v>
       </c>
@@ -5886,7 +5976,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
         <v>318</v>
       </c>
@@ -5894,7 +5984,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
         <v>319</v>
       </c>
@@ -5902,1813 +5992,2119 @@
         <v>304</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A125" s="12" t="s">
-        <v>207</v>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A125" s="1" t="s">
+        <v>351</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="C125" s="12" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A126" s="12" t="s">
-        <v>210</v>
+        <v>304</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A126" s="1" t="s">
+        <v>352</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="C126" s="12" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A127" s="12" t="s">
-        <v>211</v>
+        <v>304</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A127" s="1" t="s">
+        <v>353</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="C127" s="12" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>212</v>
+        <v>310</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="C128" s="1" t="s">
-        <v>213</v>
+        <v>304</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>214</v>
+        <v>354</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="C129" s="1" t="s">
-        <v>213</v>
+        <v>304</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>215</v>
+        <v>305</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>300</v>
-      </c>
-      <c r="C130" s="1" t="s">
-        <v>213</v>
+        <v>304</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="B131" t="s">
-        <v>302</v>
-      </c>
-      <c r="C131" t="s">
-        <v>289</v>
+        <v>316</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="B132" t="s">
-        <v>302</v>
-      </c>
-      <c r="C132" t="s">
-        <v>291</v>
+        <v>355</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="B133" t="s">
-        <v>302</v>
-      </c>
-      <c r="C133" t="s">
-        <v>293</v>
+        <v>356</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B134" t="s">
-        <v>302</v>
-      </c>
-      <c r="C134" t="s">
-        <v>293</v>
+        <v>357</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="B135" t="s">
-        <v>302</v>
-      </c>
-      <c r="C135" t="s">
-        <v>296</v>
+        <v>358</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A136" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="B136" t="s">
-        <v>302</v>
-      </c>
-      <c r="C136" t="s">
-        <v>296</v>
+      <c r="A136" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C136" s="12" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A137" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="B137" t="s">
-        <v>302</v>
-      </c>
-      <c r="C137" t="s">
-        <v>296</v>
+      <c r="A137" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C137" s="12" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A138" s="1" t="s">
-        <v>126</v>
+      <c r="A138" s="12" t="s">
+        <v>211</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C138" s="1" t="s">
-        <v>128</v>
+        <v>300</v>
+      </c>
+      <c r="C138" s="12" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>129</v>
+        <v>212</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>127</v>
+        <v>300</v>
       </c>
       <c r="C139" s="1" t="s">
-        <v>128</v>
+        <v>213</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>130</v>
+        <v>214</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>127</v>
+        <v>300</v>
       </c>
       <c r="C140" s="1" t="s">
-        <v>128</v>
+        <v>213</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>131</v>
+        <v>215</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>127</v>
+        <v>300</v>
       </c>
       <c r="C141" s="1" t="s">
-        <v>128</v>
+        <v>213</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>132</v>
+        <v>3</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>128</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="C142" s="1"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>133</v>
+        <v>331</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>134</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="C143" s="1"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>135</v>
+        <v>332</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C144" s="1" t="s">
-        <v>134</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="C144" s="1"/>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>136</v>
+        <v>7</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C145" s="1" t="s">
-        <v>134</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="C145" s="1"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>137</v>
+        <v>333</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C146" s="1" t="s">
-        <v>138</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="C146" s="1"/>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" s="1" t="s">
-        <v>139</v>
+        <v>334</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C147" s="1" t="s">
-        <v>138</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="C147" s="1"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="1" t="s">
-        <v>140</v>
+        <v>335</v>
       </c>
       <c r="B148" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C148" s="1" t="s">
-        <v>138</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="C148" s="1"/>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="1" t="s">
-        <v>141</v>
+        <v>330</v>
       </c>
       <c r="B149" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C149" s="1" t="s">
-        <v>138</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="C149" s="1"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="1" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B150" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C150" s="1" t="s">
-        <v>142</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="C150" s="1"/>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" s="1" t="s">
-        <v>25</v>
+        <v>329</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C151" s="1" t="s">
-        <v>142</v>
-      </c>
+        <v>302</v>
+      </c>
+      <c r="C151" s="1"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B152" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C152" s="1" t="s">
-        <v>142</v>
+        <v>288</v>
+      </c>
+      <c r="B152" t="s">
+        <v>302</v>
+      </c>
+      <c r="C152" t="s">
+        <v>289</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B153" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>142</v>
+        <v>290</v>
+      </c>
+      <c r="B153" t="s">
+        <v>302</v>
+      </c>
+      <c r="C153" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C154" s="1" t="s">
-        <v>142</v>
+        <v>292</v>
+      </c>
+      <c r="B154" t="s">
+        <v>302</v>
+      </c>
+      <c r="C154" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B155" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C155" s="1" t="s">
-        <v>142</v>
+        <v>294</v>
+      </c>
+      <c r="B155" t="s">
+        <v>302</v>
+      </c>
+      <c r="C155" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C156" s="1" t="s">
-        <v>146</v>
+        <v>295</v>
+      </c>
+      <c r="B156" t="s">
+        <v>302</v>
+      </c>
+      <c r="C156" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C157" s="1" t="s">
-        <v>146</v>
+        <v>297</v>
+      </c>
+      <c r="B157" t="s">
+        <v>302</v>
+      </c>
+      <c r="C157" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B158" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C158" s="1" t="s">
-        <v>146</v>
+        <v>298</v>
+      </c>
+      <c r="B158" t="s">
+        <v>302</v>
+      </c>
+      <c r="C158" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" s="1" t="s">
-        <v>149</v>
+        <v>126</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C159" s="1" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="1" t="s">
-        <v>150</v>
+        <v>129</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C160" s="1" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
-        <v>151</v>
+        <v>130</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
-        <v>153</v>
+        <v>132</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
-        <v>154</v>
+        <v>133</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>157</v>
+        <v>134</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C170" s="1" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
-        <v>163</v>
+        <v>28</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
-        <v>164</v>
+        <v>25</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
-        <v>165</v>
+        <v>26</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C173" s="1" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
-        <v>10</v>
+        <v>27</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C174" s="1" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C175" s="1" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C176" s="1" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
-        <v>169</v>
+        <v>145</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C177" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
-        <v>170</v>
+        <v>147</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
-        <v>171</v>
+        <v>148</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
-        <v>173</v>
+        <v>149</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C180" s="1" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
-        <v>174</v>
+        <v>150</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
-        <v>175</v>
+        <v>151</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>176</v>
+        <v>146</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
-        <v>177</v>
+        <v>145</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
-        <v>178</v>
+        <v>153</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
-        <v>179</v>
+        <v>154</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
-        <v>180</v>
+        <v>155</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>176</v>
+        <v>152</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
-        <v>181</v>
+        <v>156</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C187" s="1" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
-        <v>183</v>
+        <v>158</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
-        <v>184</v>
+        <v>159</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C189" s="1" t="s">
-        <v>182</v>
+        <v>157</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
-        <v>185</v>
+        <v>160</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
-        <v>186</v>
+        <v>162</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>188</v>
+        <v>163</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" s="1" t="s">
-        <v>189</v>
+        <v>164</v>
       </c>
       <c r="B193" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" s="1" t="s">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" s="1" t="s">
-        <v>191</v>
+        <v>10</v>
       </c>
       <c r="B195" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" s="1" t="s">
-        <v>192</v>
+        <v>167</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" s="1" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" s="1" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>193</v>
+        <v>166</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A199" s="11" t="s">
-        <v>196</v>
+      <c r="A199" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="B199" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C199" s="11" t="s">
-        <v>197</v>
+      <c r="C199" s="1" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A200" s="11" t="s">
-        <v>10</v>
+      <c r="A200" s="1" t="s">
+        <v>171</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C200" s="11" t="s">
-        <v>197</v>
+      <c r="C200" s="1" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A201" s="11" t="s">
-        <v>141</v>
+      <c r="A201" s="1" t="s">
+        <v>173</v>
       </c>
       <c r="B201" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C201" s="11" t="s">
-        <v>197</v>
+      <c r="C201" s="1" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A202" s="11" t="s">
-        <v>198</v>
+      <c r="A202" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="B202" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C202" s="11" t="s">
-        <v>197</v>
+      <c r="C202" s="1" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A203" s="11" t="s">
-        <v>199</v>
+      <c r="A203" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="B203" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C203" s="11" t="s">
-        <v>197</v>
+      <c r="C203" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A204" s="11" t="s">
-        <v>200</v>
+      <c r="A204" s="1" t="s">
+        <v>177</v>
       </c>
       <c r="B204" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C204" s="11" t="s">
-        <v>197</v>
+      <c r="C204" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A205" s="11" t="s">
-        <v>201</v>
+      <c r="A205" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="B205" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C205" s="11" t="s">
-        <v>197</v>
+      <c r="C205" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A206" s="11" t="s">
-        <v>202</v>
+      <c r="A206" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C206" s="11" t="s">
-        <v>197</v>
+      <c r="C206" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A207" s="11" t="s">
-        <v>203</v>
+      <c r="A207" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="B207" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C207" s="11" t="s">
-        <v>197</v>
+      <c r="C207" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A208" s="11" t="s">
-        <v>204</v>
+      <c r="A208" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C208" s="11" t="s">
-        <v>197</v>
+      <c r="C208" s="1" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A209" s="11" t="s">
-        <v>205</v>
+      <c r="A209" s="1" t="s">
+        <v>183</v>
       </c>
       <c r="B209" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C209" s="11" t="s">
-        <v>197</v>
+      <c r="C209" s="1" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A210" s="11" t="s">
-        <v>328</v>
+      <c r="A210" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="B210" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C210" s="11"/>
+      <c r="C210" s="1" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A211" s="11" t="s">
-        <v>247</v>
+      <c r="A211" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="B211" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C211" s="11"/>
+      <c r="C211" s="1" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A212" s="11" t="s">
-        <v>272</v>
+      <c r="A212" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="B212" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C212" s="11"/>
+      <c r="C212" s="1" t="s">
+        <v>187</v>
+      </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" s="1" t="s">
-        <v>320</v>
+        <v>188</v>
       </c>
       <c r="B213" s="1" t="s">
         <v>127</v>
+      </c>
+      <c r="C213" s="1" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214" s="1" t="s">
-        <v>321</v>
+        <v>189</v>
       </c>
       <c r="B214" s="1" t="s">
         <v>127</v>
+      </c>
+      <c r="C214" s="1" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215" s="1" t="s">
-        <v>322</v>
+        <v>190</v>
       </c>
       <c r="B215" s="1" t="s">
         <v>127</v>
+      </c>
+      <c r="C215" s="1" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" s="1" t="s">
-        <v>323</v>
+        <v>191</v>
       </c>
       <c r="B216" s="1" t="s">
         <v>127</v>
+      </c>
+      <c r="C216" s="1" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217" s="1" t="s">
-        <v>324</v>
+        <v>192</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>127</v>
+      </c>
+      <c r="C217" s="1" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A218" s="1" t="s">
-        <v>325</v>
+        <v>194</v>
       </c>
       <c r="B218" s="1" t="s">
         <v>127</v>
+      </c>
+      <c r="C218" s="1" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A219" s="1" t="s">
-        <v>326</v>
+        <v>195</v>
       </c>
       <c r="B219" s="1" t="s">
         <v>127</v>
       </c>
+      <c r="C219" s="1" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A220" s="1" t="s">
-        <v>327</v>
+      <c r="A220" s="11" t="s">
+        <v>196</v>
       </c>
       <c r="B220" s="1" t="s">
         <v>127</v>
       </c>
+      <c r="C220" s="11" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A221" s="1" t="s">
-        <v>163</v>
+      <c r="A221" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="B221" s="1" t="s">
         <v>127</v>
       </c>
+      <c r="C221" s="11" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A222" s="1" t="s">
-        <v>175</v>
+      <c r="A222" s="11" t="s">
+        <v>141</v>
       </c>
       <c r="B222" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C222" s="1" t="s">
-        <v>176</v>
+        <v>127</v>
+      </c>
+      <c r="C222" s="11" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A223" s="1" t="s">
-        <v>177</v>
+      <c r="A223" s="11" t="s">
+        <v>198</v>
       </c>
       <c r="B223" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C223" s="1" t="s">
-        <v>176</v>
+        <v>127</v>
+      </c>
+      <c r="C223" s="11" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A224" s="1" t="s">
-        <v>178</v>
+      <c r="A224" s="11" t="s">
+        <v>199</v>
       </c>
       <c r="B224" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C224" s="1" t="s">
-        <v>176</v>
+        <v>127</v>
+      </c>
+      <c r="C224" s="11" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A225" s="1" t="s">
-        <v>179</v>
+      <c r="A225" s="11" t="s">
+        <v>200</v>
       </c>
       <c r="B225" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C225" s="1" t="s">
-        <v>176</v>
+        <v>127</v>
+      </c>
+      <c r="C225" s="11" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A226" s="1" t="s">
-        <v>180</v>
+      <c r="A226" s="11" t="s">
+        <v>201</v>
       </c>
       <c r="B226" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C226" s="1" t="s">
-        <v>176</v>
+        <v>127</v>
+      </c>
+      <c r="C226" s="11" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A227" s="1" t="s">
-        <v>217</v>
+      <c r="A227" s="11" t="s">
+        <v>202</v>
       </c>
       <c r="B227" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C227" s="1" t="s">
-        <v>176</v>
+        <v>127</v>
+      </c>
+      <c r="C227" s="11" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A228" s="1" t="s">
-        <v>218</v>
+      <c r="A228" s="11" t="s">
+        <v>203</v>
       </c>
       <c r="B228" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C228" s="1" t="s">
-        <v>176</v>
+        <v>127</v>
+      </c>
+      <c r="C228" s="11" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A229" s="1" t="s">
-        <v>219</v>
+      <c r="A229" s="11" t="s">
+        <v>204</v>
       </c>
       <c r="B229" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C229" s="1" t="s">
-        <v>176</v>
+        <v>127</v>
+      </c>
+      <c r="C229" s="11" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A230" s="1" t="s">
-        <v>220</v>
+      <c r="A230" s="11" t="s">
+        <v>205</v>
       </c>
       <c r="B230" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C230" s="1" t="s">
-        <v>176</v>
+        <v>127</v>
+      </c>
+      <c r="C230" s="11" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A231" s="1" t="s">
-        <v>221</v>
+      <c r="A231" s="11" t="s">
+        <v>328</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C231" s="1" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="232" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A232" s="14" t="s">
-        <v>170</v>
+        <v>127</v>
+      </c>
+      <c r="C231" s="11"/>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A232" s="11" t="s">
+        <v>247</v>
       </c>
       <c r="B232" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C232" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="233" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A233" s="14" t="s">
-        <v>223</v>
+        <v>127</v>
+      </c>
+      <c r="C232" s="11"/>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A233" s="11" t="s">
+        <v>272</v>
       </c>
       <c r="B233" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C233" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="234" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A234" s="14" t="s">
-        <v>224</v>
+        <v>127</v>
+      </c>
+      <c r="C233" s="11"/>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A234" s="1" t="s">
+        <v>320</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C234" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="235" spans="1:3" ht="19" x14ac:dyDescent="0.2">
-      <c r="A235" s="14" t="s">
-        <v>225</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A235" s="1" t="s">
+        <v>321</v>
       </c>
       <c r="B235" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C235" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="236" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A236" s="15" t="s">
-        <v>226</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A236" s="1" t="s">
+        <v>322</v>
       </c>
       <c r="B236" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C236" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="237" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A237" s="15" t="s">
-        <v>227</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A237" s="1" t="s">
+        <v>323</v>
       </c>
       <c r="B237" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C237" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="238" spans="1:3" ht="18" x14ac:dyDescent="0.2">
-      <c r="A238" s="15" t="s">
-        <v>229</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A238" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="B238" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C238" t="s">
-        <v>230</v>
+        <v>127</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
-        <v>231</v>
+        <v>325</v>
       </c>
       <c r="B239" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C239" t="s">
-        <v>13</v>
+        <v>127</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
-        <v>232</v>
+        <v>326</v>
       </c>
       <c r="B240" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C240" t="s">
-        <v>13</v>
+        <v>127</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
-        <v>9</v>
+        <v>327</v>
       </c>
       <c r="B241" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C241" t="s">
-        <v>13</v>
+        <v>127</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
-        <v>233</v>
+        <v>163</v>
       </c>
       <c r="B242" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="C242" t="s">
-        <v>13</v>
+        <v>127</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
-        <v>234</v>
+        <v>175</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C243" t="s">
-        <v>13</v>
+      <c r="C243" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
-        <v>235</v>
+        <v>177</v>
       </c>
       <c r="B244" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C244" t="s">
-        <v>13</v>
+      <c r="C244" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
-        <v>236</v>
+        <v>178</v>
       </c>
       <c r="B245" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C245" t="s">
-        <v>13</v>
+      <c r="C245" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
-        <v>237</v>
+        <v>179</v>
       </c>
       <c r="B246" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C246" t="s">
-        <v>13</v>
+      <c r="C246" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
-        <v>238</v>
+        <v>180</v>
       </c>
       <c r="B247" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C247" t="s">
-        <v>13</v>
+      <c r="C247" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
-        <v>239</v>
+        <v>217</v>
       </c>
       <c r="B248" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C248" t="s">
-        <v>13</v>
+      <c r="C248" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
-        <v>240</v>
+        <v>218</v>
       </c>
       <c r="B249" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C249" t="s">
-        <v>13</v>
+      <c r="C249" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
       <c r="B250" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C250" t="s">
-        <v>13</v>
+      <c r="C250" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
-        <v>242</v>
+        <v>220</v>
       </c>
       <c r="B251" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C251" t="s">
-        <v>13</v>
+      <c r="C251" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
-        <v>243</v>
+        <v>221</v>
       </c>
       <c r="B252" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="C252" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A253" s="1" t="s">
-        <v>244</v>
+      <c r="C252" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A253" s="14" t="s">
+        <v>170</v>
       </c>
       <c r="B253" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C253" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A254" s="1" t="s">
-        <v>246</v>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A254" s="14" t="s">
+        <v>223</v>
       </c>
       <c r="B254" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C254" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A255" s="1" t="s">
-        <v>247</v>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A255" s="14" t="s">
+        <v>224</v>
       </c>
       <c r="B255" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C255" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A256" s="1" t="s">
-        <v>248</v>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A256" s="14" t="s">
+        <v>225</v>
       </c>
       <c r="B256" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C256" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="257" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A257" s="1" t="s">
-        <v>249</v>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A257" s="15" t="s">
+        <v>226</v>
       </c>
       <c r="B257" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C257" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="258" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A258" s="1" t="s">
-        <v>250</v>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A258" s="15" t="s">
+        <v>227</v>
       </c>
       <c r="B258" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C258" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A259" s="1" t="s">
-        <v>251</v>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A259" s="15" t="s">
+        <v>229</v>
       </c>
       <c r="B259" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C259" t="s">
-        <v>245</v>
+        <v>230</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" s="1" t="s">
-        <v>252</v>
+        <v>231</v>
       </c>
       <c r="B260" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C260" t="s">
-        <v>245</v>
+        <v>13</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" s="1" t="s">
-        <v>253</v>
+        <v>232</v>
       </c>
       <c r="B261" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C261" t="s">
-        <v>245</v>
+        <v>13</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" s="1" t="s">
-        <v>254</v>
+        <v>9</v>
       </c>
       <c r="B262" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C262" t="s">
-        <v>245</v>
+        <v>13</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" s="1" t="s">
-        <v>255</v>
+        <v>233</v>
       </c>
       <c r="B263" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C263" t="s">
-        <v>245</v>
+        <v>13</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264" s="1" t="s">
-        <v>256</v>
+        <v>234</v>
       </c>
       <c r="B264" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C264" t="s">
-        <v>245</v>
+        <v>13</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A265" s="1" t="s">
-        <v>257</v>
+        <v>235</v>
       </c>
       <c r="B265" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C265" t="s">
-        <v>245</v>
+        <v>13</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A266" s="1" t="s">
-        <v>258</v>
+        <v>236</v>
       </c>
       <c r="B266" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C266" t="s">
-        <v>245</v>
+        <v>13</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" s="1" t="s">
-        <v>259</v>
+        <v>237</v>
       </c>
       <c r="B267" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C267" t="s">
-        <v>245</v>
+        <v>13</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" s="1" t="s">
-        <v>260</v>
+        <v>238</v>
       </c>
       <c r="B268" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C268" t="s">
-        <v>245</v>
+        <v>13</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269" s="1" t="s">
-        <v>261</v>
+        <v>239</v>
       </c>
       <c r="B269" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C269" t="s">
-        <v>245</v>
+        <v>13</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270" s="1" t="s">
-        <v>262</v>
+        <v>240</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C270" t="s">
-        <v>245</v>
+        <v>13</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" s="1" t="s">
-        <v>263</v>
+        <v>241</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C271" t="s">
-        <v>245</v>
+        <v>13</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272" s="1" t="s">
-        <v>264</v>
+        <v>242</v>
       </c>
       <c r="B272" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C272" t="s">
-        <v>245</v>
+        <v>13</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A273" s="1" t="s">
-        <v>265</v>
+        <v>243</v>
       </c>
       <c r="B273" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C273" t="s">
-        <v>266</v>
+        <v>13</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A274" s="1" t="s">
-        <v>267</v>
+        <v>244</v>
       </c>
       <c r="B274" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C274" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A275" s="1" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="B275" s="1" t="s">
         <v>216</v>
       </c>
       <c r="C275" t="s">
-        <v>266</v>
+        <v>245</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A276" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="B276" t="s">
-        <v>301</v>
+        <v>247</v>
+      </c>
+      <c r="B276" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C276" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="B277" t="s">
-        <v>301</v>
+        <v>248</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C277" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="B278" t="s">
-        <v>301</v>
+        <v>249</v>
+      </c>
+      <c r="B278" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C278" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A279" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="B279" t="s">
-        <v>301</v>
+        <v>250</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C279" t="s">
-        <v>274</v>
+        <v>245</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="B280" t="s">
-        <v>301</v>
+        <v>251</v>
+      </c>
+      <c r="B280" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C280" t="s">
-        <v>274</v>
+        <v>245</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="B281" t="s">
-        <v>301</v>
+        <v>252</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C281" t="s">
-        <v>274</v>
+        <v>245</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282" s="1" t="s">
-        <v>277</v>
-      </c>
-      <c r="B282" t="s">
-        <v>301</v>
+        <v>253</v>
+      </c>
+      <c r="B282" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C282" t="s">
-        <v>274</v>
+        <v>245</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B283" t="s">
-        <v>301</v>
+        <v>254</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C283" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="B284" t="s">
-        <v>301</v>
+        <v>255</v>
+      </c>
+      <c r="B284" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C284" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="B285" t="s">
-        <v>301</v>
+        <v>256</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C285" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="B286" t="s">
-        <v>301</v>
+        <v>257</v>
+      </c>
+      <c r="B286" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C286" t="s">
-        <v>278</v>
+        <v>245</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="B287" t="s">
-        <v>301</v>
+        <v>258</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C287" t="s">
-        <v>283</v>
+        <v>245</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="B288" t="s">
-        <v>301</v>
+        <v>259</v>
+      </c>
+      <c r="B288" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C288" t="s">
-        <v>283</v>
+        <v>245</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A289" s="1" t="s">
-        <v>285</v>
-      </c>
-      <c r="B289" t="s">
-        <v>301</v>
+        <v>260</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C289" t="s">
-        <v>283</v>
+        <v>245</v>
       </c>
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A290" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="B290" t="s">
-        <v>301</v>
+        <v>261</v>
+      </c>
+      <c r="B290" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C290" t="s">
-        <v>283</v>
+        <v>245</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A291" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C291" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A292" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="B292" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C292" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A293" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C293" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A294" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B294" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C294" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A295" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="B295" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C295" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A296" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="B296" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C296" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A297" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="B297" t="s">
+        <v>301</v>
+      </c>
+      <c r="C297" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A298" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="B298" t="s">
+        <v>301</v>
+      </c>
+      <c r="C298" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A299" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="B299" t="s">
+        <v>301</v>
+      </c>
+      <c r="C299" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A300" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="B300" t="s">
+        <v>301</v>
+      </c>
+      <c r="C300" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A301" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="B301" t="s">
+        <v>301</v>
+      </c>
+      <c r="C301" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A302" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="B302" t="s">
+        <v>301</v>
+      </c>
+      <c r="C302" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A303" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B303" t="s">
+        <v>301</v>
+      </c>
+      <c r="C303" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A304" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B304" t="s">
+        <v>301</v>
+      </c>
+      <c r="C304" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A305" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="B305" t="s">
+        <v>301</v>
+      </c>
+      <c r="C305" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A306" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="B306" t="s">
+        <v>301</v>
+      </c>
+      <c r="C306" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A307" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="B307" t="s">
+        <v>301</v>
+      </c>
+      <c r="C307" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A308" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="B308" t="s">
+        <v>301</v>
+      </c>
+      <c r="C308" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A309" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B309" t="s">
+        <v>301</v>
+      </c>
+      <c r="C309" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A310" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B310" t="s">
+        <v>301</v>
+      </c>
+      <c r="C310" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A311" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B311" t="s">
+        <v>301</v>
+      </c>
+      <c r="C311" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A312" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B291" t="s">
+      <c r="B312" t="s">
         <v>301</v>
       </c>
-      <c r="C291" t="s">
+      <c r="C312" t="s">
         <v>283</v>
       </c>
     </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A313" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B313" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A314" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="B314" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A315" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B315" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A316" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="B316" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A317" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B317" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A318" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B318" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A319" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="B319" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A320" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B320" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A321" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="B321" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A322" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="B322" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A323" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B323" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A324" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="B324" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A325" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B325" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A326" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="B326" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A327" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B327" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A328" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B328" t="s">
+        <v>301</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C291">
-    <sortCondition ref="B2:B291"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C312">
+    <sortCondition ref="B2:B312"/>
   </sortState>
   <hyperlinks>
     <hyperlink ref="A29" r:id="rId1" xr:uid="{00000000-0004-0000-0600-000000000000}"/>

</xml_diff>